<commit_message>
deleted unneceassary lld classes
</commit_message>
<xml_diff>
--- a/lld/LLD.xlsx
+++ b/lld/LLD.xlsx
@@ -8,19 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Interview_Preparations\LLD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A99BCB2-922B-4728-A6C5-04AC89AC3642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71AE5D26-897F-4E0A-8CFC-33F635437124}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{8CD57D6A-E751-493E-AE1E-40EC8EBC696F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="918" xr2:uid="{8CD57D6A-E751-493E-AE1E-40EC8EBC696F}"/>
   </bookViews>
   <sheets>
     <sheet name="Interview_Preparation" sheetId="4" r:id="rId1"/>
     <sheet name="LLD Questions" sheetId="2" r:id="rId2"/>
     <sheet name=" HLD Questions" sheetId="3" r:id="rId3"/>
-    <sheet name="InterviewDetails" sheetId="5" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="7" r:id="rId5"/>
-    <sheet name="Sheet3" sheetId="8" r:id="rId6"/>
+    <sheet name="Questions_Patteren" sheetId="9" r:id="rId4"/>
+    <sheet name="InterviewDetails" sheetId="5" r:id="rId5"/>
+    <sheet name="Companiees" sheetId="7" r:id="rId6"/>
+    <sheet name="MansiCollege" sheetId="10" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="269">
   <si>
     <t>Dynamic Programming</t>
   </si>
@@ -522,18 +524,6 @@
     <t>Sorting and Searching</t>
   </si>
   <si>
-    <t>Letter Combinations of a Phone Number</t>
-  </si>
-  <si>
-    <t>Generate Parentheses</t>
-  </si>
-  <si>
-    <t>Word Search</t>
-  </si>
-  <si>
-    <t>Word Search II</t>
-  </si>
-  <si>
     <t>Others</t>
   </si>
   <si>
@@ -552,9 +542,6 @@
     <t>O(N+K)</t>
   </si>
   <si>
-    <t>K Closest Points to Origin - https://leetcode.com/problems/k-closest-points-to-origin/submissions/</t>
-  </si>
-  <si>
     <t>Meeting Rooms II - https://leetcode.com/problems/meeting-rooms-ii/</t>
   </si>
   <si>
@@ -576,9 +563,6 @@
     <t>Reverse Integer - https://leetcode.com/problems/reverse-integer/solution/</t>
   </si>
   <si>
-    <t>Second Highest Salary - https://leetcode.com/explore/interview/card/amazon/82/others/3003/</t>
-  </si>
-  <si>
     <t>Two Sum II - Input array is sorted - https://leetcode.com/problems/two-sum-ii-input-array-is-sorted/</t>
   </si>
   <si>
@@ -598,9 +582,6 @@
   </si>
   <si>
     <t>Serialize and Deserialize Binary Tree : https://leetcode.com/problems/serialize-and-deserialize-binary-tree/solution/</t>
-  </si>
-  <si>
-    <t>Maximum Frequency Stack</t>
   </si>
   <si>
     <t>Rotting Oranges https://leetcode.com/problems/rotting-oranges/</t>
@@ -707,9 +688,6 @@
     <t xml:space="preserve">VMWare </t>
   </si>
   <si>
-    <t>Scheduled</t>
-  </si>
-  <si>
     <t>Sigmoid Analytics</t>
   </si>
   <si>
@@ -728,16 +706,10 @@
     <t>Kth Smallest Element in a BST - https://leetcode.com/problems/kth-smallest-element-in-a-bst/</t>
   </si>
   <si>
-    <t>O(H+K)</t>
-  </si>
-  <si>
     <t>HeightOfABinaryTree - https://www.techiedelight.com/calculate-height-binary-tree-iterative-recursive/</t>
   </si>
   <si>
     <t>ClimbingStairs - https://leetcode.com/problems/climbing-stairs/solution/</t>
-  </si>
-  <si>
-    <t>LongestIncreasingSubsequence - https://leetcode.com/problems/longest-increasing-subsequence/</t>
   </si>
   <si>
     <r>
@@ -790,9 +762,6 @@
     <t>Search a 2D Matrix - https://leetcode.com/problems/search-a-2d-matrix/</t>
   </si>
   <si>
-    <t>O(NLOGN)</t>
-  </si>
-  <si>
     <t>O(Log(M*N))</t>
   </si>
   <si>
@@ -880,29 +849,341 @@
     <t>Design Twitter</t>
   </si>
   <si>
-    <t>Median of Two Sorted Arrays - https://leetcode.com/explore/interview/card/amazon/79/sorting-and-searching/2991/</t>
-  </si>
-  <si>
-    <t>O(log(m,n))</t>
-  </si>
-  <si>
-    <t>Kth Largest Element in a BST - https://leetcode.com/problems/kth-smallest-element-in-a-bst/</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
     <t>Design Dropbox</t>
+  </si>
+  <si>
+    <t>O(K)</t>
+  </si>
+  <si>
+    <t>Kth Largest Element in a BST - same as Kth Smallest Element in a BST</t>
+  </si>
+  <si>
+    <t>Hard</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">LongestIncreasingSubsequence - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>https://le</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>etcode.com/problems/longest-increasing-subsequence/</t>
+    </r>
+  </si>
+  <si>
+    <t>Longest Common Subsequence - https://leetcode.com/problems/longest-common-subsequence/solution/</t>
+  </si>
+  <si>
+    <t>Reverse Words in a String - https://leetcode.com/problems/reverse-words-in-a-string/submissions/</t>
+  </si>
+  <si>
+    <t>Valid Palindrome - https://leetcode.com/problems/valid-palindrome/</t>
+  </si>
+  <si>
+    <t>Set Matrix Zeroes- https://leetcode.com/explore/interview/card/microsoft/30/array-and-strings/203/</t>
+  </si>
+  <si>
+    <t>If input array is sorted then</t>
+  </si>
+  <si>
+    <t>- Two pointers</t>
+  </si>
+  <si>
+    <t>If asked for all permutations/subsets then</t>
+  </si>
+  <si>
+    <t>If given a tree then</t>
+  </si>
+  <si>
+    <t>- DFS</t>
+  </si>
+  <si>
+    <t>- BFS</t>
+  </si>
+  <si>
+    <t>If given a graph then</t>
+  </si>
+  <si>
+    <t>If given a linked list then</t>
+  </si>
+  <si>
+    <t>If recursion is banned then</t>
+  </si>
+  <si>
+    <t>- Stack</t>
+  </si>
+  <si>
+    <t>If must solve in-place then</t>
+  </si>
+  <si>
+    <t>- Swap corresponding values</t>
+  </si>
+  <si>
+    <t>- Store one or more different values in the same pointer</t>
+  </si>
+  <si>
+    <t>If asked for maximum/minimum subarray/subset/options then</t>
+  </si>
+  <si>
+    <t>- Dynamic programming</t>
+  </si>
+  <si>
+    <t>If asked for top/least K items then</t>
+  </si>
+  <si>
+    <t>- Heap</t>
+  </si>
+  <si>
+    <t>If asked for common strings then</t>
+  </si>
+  <si>
+    <t>- Map</t>
+  </si>
+  <si>
+    <t>- Trie</t>
+  </si>
+  <si>
+    <t>Else</t>
+  </si>
+  <si>
+    <t>- Map/Set for O(1) time &amp; O(n) space</t>
+  </si>
+  <si>
+    <t>- Sort input for O(nlogn) time and O(1) space</t>
+  </si>
+  <si>
+    <t>O(T*N)</t>
+  </si>
+  <si>
+    <t>O(T)</t>
+  </si>
+  <si>
+    <t>College Name</t>
+  </si>
+  <si>
+    <t>St. Ann's College For Women</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fee Structure </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Admission </t>
+  </si>
+  <si>
+    <t>Percentage Should be greator than 70%</t>
+  </si>
+  <si>
+    <t>The Indian Institute of Management and Commerce(IIMC)</t>
+  </si>
+  <si>
+    <t>Based upon percentage last year cut off 89%</t>
+  </si>
+  <si>
+    <t>Binary search</t>
+  </si>
+  <si>
+    <t>Two pointers</t>
+  </si>
+  <si>
+    <t>Backtracking</t>
+  </si>
+  <si>
+    <t>Vishwa Vishwani Institute of Systems &amp; Management Office, Stanza Building, Flat #601,mahavir Chambers, Liberty X Road, Himayatnagar, Hyderabad, Telangana 500029</t>
+  </si>
+  <si>
+    <t>1Lac+</t>
+  </si>
+  <si>
+    <t>London Management Academy</t>
+  </si>
+  <si>
+    <t>₹1.2 Lakhs (1st Year Fees)</t>
+  </si>
+  <si>
+    <t>70% - Accoring to 12th percentage</t>
+  </si>
+  <si>
+    <t>Longest Substring with At Most K Distinct Characters https://leetcode.com/problems/longest-substring-with-at-most-k-distinct-characters/solution/</t>
+  </si>
+  <si>
+    <t>Tech Mojo</t>
+  </si>
+  <si>
+    <t>PayU</t>
+  </si>
+  <si>
+    <t>Combination Sum IV - https://leetcode.com/problems/combination-sum-iv/</t>
+  </si>
+  <si>
+    <t>Unique Paths - https://leetcode.com/problems/unique-paths/submissions/</t>
+  </si>
+  <si>
+    <t>Jump Game - https://leetcode.com/problems/jump-game/</t>
+  </si>
+  <si>
+    <t>House Robber : https://leetcode.com/problems/house-robber/solution/</t>
+  </si>
+  <si>
+    <t>House Robber II - https://leetcode.com/problems/house-robber-ii/solution/</t>
+  </si>
+  <si>
+    <t>Decode Ways - https://leetcode.com/problems/decode-ways/solution/</t>
+  </si>
+  <si>
+    <t>Implement Trie (Prefix Tree) - https://leetcode.com/problems/implement-trie-prefix-tree/</t>
+  </si>
+  <si>
+    <t>Find Minimum in Rotated Sorted Array -https://leetcode.com/problems/find-minimum-in-rotated-sorted-array/</t>
+  </si>
+  <si>
+    <t>Number of Connected Components in an Undirected Graph : https://leetcode.com/problems/number-of-connected-components-in-an-undirected-graph/</t>
+  </si>
+  <si>
+    <t>Letter Combinations of a Phone Number - https://leetcode.com/problems/letter-combinations-of-a-phone-number/</t>
+  </si>
+  <si>
+    <r>
+      <t>O</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(4^N.N</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="KaTeX_Math"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Word Search - https://leetcode.com/problems/word-search/solution/</t>
+  </si>
+  <si>
+    <t>O(N.3^L)</t>
+  </si>
+  <si>
+    <t>TC - O(V+E)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SC - O(V)</t>
+  </si>
+  <si>
+    <t>O(V)</t>
+  </si>
+  <si>
+    <t>BFS -  https://www.geeksforgeeks.org/breadth-first-search-or-bfs-for-a-graph/(Queue)</t>
+  </si>
+  <si>
+    <t>DFS - https://www.geeksforgeeks.org/depth-first-search-or-dfs-for-a-graph/(Stack)</t>
+  </si>
+  <si>
+    <t>Cycle Detection In Directed Graph Using BFS</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/longest-common-prefix/ - Trie</t>
+  </si>
+  <si>
+    <t>Prim's Algo - https://practice.geeksforgeeks.org/problems/minimum-spanning-tree/1</t>
+  </si>
+  <si>
+    <t>ELogE - if we use hashmap then TC ELogV</t>
+  </si>
+  <si>
+    <t>O(V+E) - if we use hashmap then TC O(V)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Dijkstra's Algorithm</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : Given a weighted, undirected and connected graph of V vertices and E edges, Find the shortest distance of all the vertex's from the source vertex S. - https://practice.geeksforgeeks.org/problems/implementing-dijkstra-set-1-adjacency-matrix/1/# </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>d(u)+c(u,v)&lt;d(v) -- &gt; d(v)=d(u)+c(u,v)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Topological sort - Graph should be DAG - dependency of jobs
+first execute the dependent processes 
+BFS (Khan's Algo) - In degree 0 will go first into queue
+</t>
+  </si>
+  <si>
+    <t>Topological sort - Graph should be DAG - dependency of jobs
+first execute the dependent processes - DFS</t>
+  </si>
+  <si>
+    <t>Shortest Path In Undirected Graph - Dijkstra's Algorithm</t>
+  </si>
+  <si>
+    <t>TC(ELogV)</t>
+  </si>
+  <si>
+    <t>SC(V2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shortest Path In Directed Acyclic Graph - Topological sort </t>
+  </si>
+  <si>
+    <t>Kruskal Algo - https://practice.geeksforgeeks.org/problems/minimum-spanning-tree/1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1036,8 +1317,29 @@
       <family val="2"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF212121"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1065,12 +1367,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1110,7 +1406,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1134,8 +1430,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1"/>
@@ -1146,33 +1440,67 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1496,317 +1824,319 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B81B669-97F6-4C1E-B0F0-0C3645C081CC}">
-  <dimension ref="A1:C97"/>
+  <dimension ref="A1:CY120"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A112" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="A116" sqref="A116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="110" style="3" customWidth="1"/>
+    <col min="1" max="1" width="114.7265625" style="3" customWidth="1"/>
     <col min="2" max="2" width="32.6328125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="25.453125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="33.26953125" style="3" customWidth="1"/>
     <col min="4" max="16384" width="8.7265625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.5">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="30" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.5">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="29" t="s">
+      <c r="B2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.5">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B3" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="29" t="s">
+      <c r="B3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.5">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B4" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="29" t="s">
+      <c r="B4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.5">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="29" t="s">
+      <c r="B5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.5">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="29" t="s">
+      <c r="C6" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.5">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.5">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C8" s="29" t="s">
+      <c r="C8" s="6" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.5">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="C9" s="29" t="s">
+      <c r="C9" s="6" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="17.5">
-      <c r="A10" s="29" t="s">
+      <c r="A10" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C10" s="32" t="s">
+      <c r="C10" s="14" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="17.5">
+    <row r="11" spans="1:3" ht="15.5">
       <c r="A11" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>75</v>
+        <v>65</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.5">
       <c r="A12" s="6" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>66</v>
+        <v>5</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>67</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.5">
-      <c r="A13" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="B13" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="29" t="s">
+      <c r="A13" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="6" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.5">
-      <c r="A14" s="29" t="s">
-        <v>69</v>
-      </c>
-      <c r="B14" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="29" t="s">
+      <c r="A14" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.5">
-      <c r="A15" s="29" t="s">
-        <v>70</v>
-      </c>
-      <c r="B15" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="29" t="s">
+      <c r="A15" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15.5">
+      <c r="A16" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15.5">
+      <c r="A17" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C17" s="37" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15.5">
+      <c r="A18" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.5">
-      <c r="A16" s="29" t="s">
-        <v>71</v>
-      </c>
-      <c r="B16" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="29" t="s">
+    <row r="19" spans="1:3">
+      <c r="A19" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="20" t="s">
+        <v>192</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="38" t="s">
+        <v>193</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="20" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15.5">
-      <c r="A17" s="29" t="s">
-        <v>72</v>
-      </c>
-      <c r="B17" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="C17" s="29" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="15.5">
-      <c r="A18" s="29" t="s">
-        <v>73</v>
-      </c>
-      <c r="B18" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="C18" s="33" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="15.5">
-      <c r="A19" s="29" t="s">
-        <v>118</v>
-      </c>
-      <c r="B19" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="29" t="s">
+    <row r="22" spans="1:3" ht="15.5">
+      <c r="A22" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C22" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="34" t="s">
-        <v>159</v>
-      </c>
-      <c r="B20" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="34" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="34" t="s">
-        <v>199</v>
-      </c>
-      <c r="B21" s="34" t="s">
-        <v>166</v>
-      </c>
-      <c r="C21" s="34" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="22"/>
-      <c r="B22" s="22"/>
-      <c r="C22" s="22"/>
-    </row>
     <row r="23" spans="1:3" ht="15.5">
-      <c r="A23" s="27" t="s">
+      <c r="A23" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" s="28" customFormat="1" ht="29">
+      <c r="A24" s="44" t="s">
+        <v>235</v>
+      </c>
+      <c r="B24" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="39" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" s="28" customFormat="1" ht="15.5">
+      <c r="A25" s="44"/>
+      <c r="B25" s="39">
+        <v>23</v>
+      </c>
+      <c r="C25" s="39"/>
+    </row>
+    <row r="26" spans="1:3" ht="15.5">
+      <c r="A26" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="B23" s="28" t="s">
+      <c r="B26" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="C23" s="28" t="s">
+      <c r="C26" s="30" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="15.5">
-      <c r="A24" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="15.5">
-      <c r="A25" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="15.5">
-      <c r="A26" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="15.5">
       <c r="A27" s="6" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>5</v>
+        <v>80</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>5</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15.5">
       <c r="A28" s="6" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>5</v>
+        <v>83</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>2</v>
@@ -1814,10 +2144,10 @@
     </row>
     <row r="29" spans="1:3" ht="15.5">
       <c r="A29" s="6" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>2</v>
@@ -1825,18 +2155,18 @@
     </row>
     <row r="30" spans="1:3" ht="15.5">
       <c r="A30" s="6" t="s">
-        <v>139</v>
+        <v>86</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>140</v>
+        <v>5</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15.5">
       <c r="A31" s="6" t="s">
-        <v>141</v>
+        <v>85</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>5</v>
@@ -1845,80 +2175,82 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="31">
-      <c r="A32" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="B32" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="C32" s="23" t="s">
+    <row r="32" spans="1:3" ht="15.5">
+      <c r="A32" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="C32" s="6" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15.5">
       <c r="A33" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="B33" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="C33" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="C33" s="6" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="15.5">
-      <c r="A34" s="22"/>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-    </row>
-    <row r="35" spans="1:3" ht="15.5">
-      <c r="A35" s="27" t="s">
+      <c r="A34" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="31">
+      <c r="A35" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="B35" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" s="39" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="15.5">
+      <c r="A36" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="B36" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" s="39" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" s="28" customFormat="1" ht="15.5">
+      <c r="A37" s="20"/>
+      <c r="B37" s="6">
+        <v>33</v>
+      </c>
+      <c r="C37" s="6"/>
+    </row>
+    <row r="38" spans="1:3" s="28" customFormat="1" ht="15.5">
+      <c r="A38" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="B35" s="28" t="s">
+      <c r="B38" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="C35" s="28" t="s">
+      <c r="C38" s="30" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="17.5">
-      <c r="A36" s="14" t="s">
+    <row r="39" spans="1:3" ht="17.5">
+      <c r="A39" s="14" t="s">
         <v>15</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="15.5">
-      <c r="A37" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="15.5">
-      <c r="A38" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B38" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="15.5">
-      <c r="A39" s="24" t="s">
-        <v>18</v>
       </c>
       <c r="B39" s="6" t="s">
         <v>5</v>
@@ -1929,73 +2261,73 @@
     </row>
     <row r="40" spans="1:3" ht="15.5">
       <c r="A40" s="6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B40" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="15.5">
       <c r="A41" s="6" t="s">
-        <v>55</v>
+        <v>17</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>54</v>
+        <v>5</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>54</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="15.5">
-      <c r="A42" s="6" t="s">
-        <v>33</v>
+      <c r="A42" s="40" t="s">
+        <v>18</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>34</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="15.5">
       <c r="A43" s="6" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="B43" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="15.5">
       <c r="A44" s="6" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>5</v>
+        <v>54</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>5</v>
+        <v>54</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="15.5">
       <c r="A45" s="6" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="15.5">
       <c r="A46" s="6" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="B46" s="6" t="s">
         <v>5</v>
@@ -2006,519 +2338,1453 @@
     </row>
     <row r="47" spans="1:3" ht="15.5">
       <c r="A47" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="15.5">
+      <c r="A48" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="15.5">
+      <c r="A49" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="15.5">
+      <c r="A50" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="15.5">
+      <c r="A51" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="15.5">
+      <c r="A52" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="15.5">
+      <c r="A53" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" s="5" customFormat="1" ht="15.5">
+      <c r="A54" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" s="5" customFormat="1" ht="15.5">
+      <c r="A55" s="25" t="s">
+        <v>148</v>
+      </c>
+      <c r="B55" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="C55" s="39" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" s="5" customFormat="1" ht="15.5">
+      <c r="A56" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="B56" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="C56" s="39" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" s="5" customFormat="1" ht="15.5">
+      <c r="A57" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="B57" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="C57" s="39" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" s="25" customFormat="1" ht="15.5">
+      <c r="A58" s="20" t="s">
+        <v>188</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" s="28" customFormat="1" ht="15.5">
+      <c r="A59" s="20" t="s">
+        <v>244</v>
+      </c>
+      <c r="B59" s="6"/>
+      <c r="C59" s="6"/>
+    </row>
+    <row r="60" spans="1:3" s="28" customFormat="1" ht="29">
+      <c r="A60" s="44" t="s">
+        <v>246</v>
+      </c>
+      <c r="B60" s="6"/>
+      <c r="C60" s="6"/>
+    </row>
+    <row r="61" spans="1:3" s="28" customFormat="1" ht="15.5">
+      <c r="A61" s="20" t="s">
+        <v>254</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" s="28" customFormat="1" ht="15.5">
+      <c r="A62" s="20" t="s">
+        <v>255</v>
+      </c>
+      <c r="B62" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" s="28" customFormat="1" ht="15.5">
+      <c r="A63" s="20"/>
+      <c r="B63" s="6">
+        <v>57</v>
+      </c>
+      <c r="C63" s="6"/>
+    </row>
+    <row r="64" spans="1:3" ht="15.5">
+      <c r="A64" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="B64" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="C64" s="30" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="15.5">
+      <c r="A65" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="B47" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C47" s="6" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="15.5">
-      <c r="A48" s="22" t="s">
-        <v>149</v>
-      </c>
-      <c r="B48" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C48" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" ht="15.5">
-      <c r="A49" s="22" t="s">
-        <v>153</v>
-      </c>
-      <c r="B49" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C49" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="15.5">
-      <c r="A50" s="22" t="s">
-        <v>150</v>
-      </c>
-      <c r="B50" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C50" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="15.5">
-      <c r="A51" s="22" t="s">
-        <v>151</v>
-      </c>
-      <c r="B51" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="C51" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" s="5" customFormat="1" ht="15.5">
-      <c r="A52" s="25" t="s">
-        <v>158</v>
-      </c>
-      <c r="B52" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="C52" s="23" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" s="5" customFormat="1" ht="15.5">
-      <c r="A53" s="22" t="s">
-        <v>117</v>
-      </c>
-      <c r="B53" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="C53" s="23" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" s="5" customFormat="1" ht="15.5">
-      <c r="A54" s="22" t="s">
-        <v>160</v>
-      </c>
-      <c r="B54" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="C54" s="23" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" s="5" customFormat="1" ht="15.5">
-      <c r="A55" s="22" t="s">
-        <v>198</v>
-      </c>
-      <c r="B55" s="23"/>
-      <c r="C55" s="23"/>
-    </row>
-    <row r="56" spans="1:3" ht="15.5">
-      <c r="A56" s="27" t="s">
-        <v>89</v>
-      </c>
-      <c r="B56" s="28" t="s">
-        <v>3</v>
-      </c>
-      <c r="C56" s="28" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="15.5">
-      <c r="A57" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="B57" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="C57" s="6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" ht="15.5">
-      <c r="A58" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="B58" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="C58" s="6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" ht="15.5">
-      <c r="A59" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="B59" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="C59" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" ht="15.5">
-      <c r="A60" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="B60" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C60" s="6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" ht="15.5">
-      <c r="A61" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="B61" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="C61" s="6" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" ht="15.5">
-      <c r="A62" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="B62" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="C62" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" ht="15.5">
-      <c r="A63" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="B63" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="C63" s="6" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" ht="15.5">
-      <c r="A64" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="B64" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="C64" s="6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" ht="15.5">
-      <c r="A65" s="26" t="s">
-        <v>163</v>
-      </c>
-      <c r="B65" s="22" t="s">
-        <v>34</v>
+      <c r="B65" s="6" t="s">
+        <v>105</v>
       </c>
       <c r="C65" s="6" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="15.5">
-      <c r="A66" s="22" t="s">
-        <v>165</v>
-      </c>
-      <c r="B66" s="22" t="s">
-        <v>167</v>
+      <c r="A66" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B66" s="6" t="s">
+        <v>97</v>
       </c>
       <c r="C66" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="15.5">
+      <c r="A67" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B67" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C67" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
-      <c r="A67" s="22"/>
-      <c r="B67" s="22"/>
-      <c r="C67" s="22"/>
-    </row>
     <row r="68" spans="1:3" ht="15.5">
-      <c r="A68" s="27" t="s">
+      <c r="A68" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B68" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="15.5">
+      <c r="A69" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B69" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C69" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="15.5">
+      <c r="A70" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B70" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C70" s="6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="15.5">
+      <c r="A71" s="41" t="s">
+        <v>153</v>
+      </c>
+      <c r="B71" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="C71" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="15.5">
+      <c r="A72" s="20" t="s">
+        <v>155</v>
+      </c>
+      <c r="B72" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="C72" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" s="28" customFormat="1">
+      <c r="A73" s="45" t="s">
+        <v>245</v>
+      </c>
+      <c r="B73" s="20"/>
+      <c r="C73" s="20"/>
+    </row>
+    <row r="74" spans="1:3" s="28" customFormat="1">
+      <c r="A74" s="20"/>
+      <c r="B74" s="20">
+        <v>64</v>
+      </c>
+      <c r="C74" s="20"/>
+    </row>
+    <row r="75" spans="1:3" ht="15.5">
+      <c r="A75" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B68" s="28" t="s">
+      <c r="B75" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="C68" s="28" t="s">
+      <c r="C75" s="30" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="17.5">
-      <c r="A69" s="14" t="s">
+    <row r="76" spans="1:3" ht="17.5">
+      <c r="A76" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B69" s="15" t="s">
+      <c r="B76" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="C69" s="7" t="s">
+      <c r="C76" s="7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="17.5">
-      <c r="A70" s="14" t="s">
+    <row r="77" spans="1:3" ht="17.5">
+      <c r="A77" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B70" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C70" s="7" t="s">
+      <c r="B77" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C77" s="7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="17.5">
-      <c r="A71" s="16" t="s">
+    <row r="78" spans="1:3" ht="17.5">
+      <c r="A78" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="B71" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C71" s="7" t="s">
+      <c r="B78" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C78" s="7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="15.5">
-      <c r="A72" s="6" t="s">
+    <row r="79" spans="1:3" s="20" customFormat="1" ht="15.5">
+      <c r="A79" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B72" s="17" t="s">
-        <v>156</v>
-      </c>
-      <c r="C72" s="7" t="s">
+      <c r="B79" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="C79" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="15.5">
+      <c r="A80" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B80" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C80" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="81" spans="1:103" ht="15.5">
+      <c r="A81" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B81" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C81" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:103" ht="15.5">
+      <c r="A82" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="B82" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C82" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:103" ht="15.5">
+      <c r="A83" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C83" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="84" spans="1:103" ht="15.5">
+      <c r="A84" s="20" t="s">
+        <v>191</v>
+      </c>
+      <c r="B84" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C84" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="85" spans="1:103" ht="15.5">
+      <c r="A85" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="B85" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="C85" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="D85" s="20"/>
+      <c r="E85" s="20"/>
+      <c r="F85" s="20"/>
+      <c r="G85" s="20"/>
+      <c r="H85" s="20"/>
+      <c r="I85" s="20"/>
+      <c r="J85" s="20"/>
+      <c r="K85" s="20"/>
+      <c r="L85" s="20"/>
+      <c r="M85" s="20"/>
+      <c r="N85" s="20"/>
+      <c r="O85" s="20"/>
+      <c r="P85" s="20"/>
+      <c r="Q85" s="20"/>
+      <c r="R85" s="20"/>
+      <c r="S85" s="20"/>
+      <c r="T85" s="20"/>
+      <c r="U85" s="20"/>
+      <c r="V85" s="20"/>
+      <c r="W85" s="20"/>
+      <c r="X85" s="20"/>
+      <c r="Y85" s="20"/>
+      <c r="Z85" s="20"/>
+      <c r="AA85" s="20"/>
+      <c r="AB85" s="20"/>
+      <c r="AC85" s="20"/>
+      <c r="AD85" s="20"/>
+      <c r="AE85" s="20"/>
+      <c r="AF85" s="20"/>
+      <c r="AG85" s="20"/>
+      <c r="AH85" s="20"/>
+      <c r="AI85" s="20"/>
+      <c r="AJ85" s="20"/>
+      <c r="AK85" s="20"/>
+      <c r="AL85" s="20"/>
+      <c r="AM85" s="20"/>
+      <c r="AN85" s="20"/>
+      <c r="AO85" s="20"/>
+      <c r="AP85" s="20"/>
+      <c r="AQ85" s="20"/>
+      <c r="AR85" s="20"/>
+      <c r="AS85" s="20"/>
+      <c r="AT85" s="20"/>
+      <c r="AU85" s="20"/>
+      <c r="AV85" s="20"/>
+      <c r="AW85" s="20"/>
+      <c r="AX85" s="20"/>
+      <c r="AY85" s="20"/>
+      <c r="AZ85" s="20"/>
+      <c r="BA85" s="20"/>
+      <c r="BB85" s="20"/>
+      <c r="BC85" s="20"/>
+      <c r="BD85" s="20"/>
+      <c r="BE85" s="20"/>
+      <c r="BF85" s="20"/>
+      <c r="BG85" s="20"/>
+      <c r="BH85" s="20"/>
+      <c r="BI85" s="20"/>
+      <c r="BJ85" s="20"/>
+      <c r="BK85" s="20"/>
+      <c r="BL85" s="20"/>
+      <c r="BM85" s="20"/>
+      <c r="BN85" s="20"/>
+      <c r="BO85" s="20"/>
+      <c r="BP85" s="20"/>
+      <c r="BQ85" s="20"/>
+      <c r="BR85" s="20"/>
+      <c r="BS85" s="20"/>
+      <c r="BT85" s="20"/>
+      <c r="BU85" s="20"/>
+      <c r="BV85" s="20"/>
+      <c r="BW85" s="20"/>
+      <c r="BX85" s="20"/>
+      <c r="BY85" s="20"/>
+      <c r="BZ85" s="20"/>
+      <c r="CA85" s="20"/>
+      <c r="CB85" s="20"/>
+      <c r="CC85" s="20"/>
+      <c r="CD85" s="20"/>
+      <c r="CE85" s="20"/>
+      <c r="CF85" s="20"/>
+      <c r="CG85" s="20"/>
+      <c r="CH85" s="20"/>
+      <c r="CI85" s="20"/>
+      <c r="CJ85" s="20"/>
+      <c r="CK85" s="20"/>
+      <c r="CL85" s="20"/>
+      <c r="CM85" s="20"/>
+      <c r="CN85" s="20"/>
+      <c r="CO85" s="20"/>
+      <c r="CP85" s="20"/>
+      <c r="CQ85" s="20"/>
+      <c r="CR85" s="20"/>
+      <c r="CS85" s="20"/>
+      <c r="CT85" s="20"/>
+      <c r="CU85" s="20"/>
+      <c r="CV85" s="20"/>
+      <c r="CW85" s="20"/>
+      <c r="CX85" s="20"/>
+      <c r="CY85" s="20"/>
+    </row>
+    <row r="86" spans="1:103" s="28" customFormat="1" ht="15.5">
+      <c r="A86" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="B86" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C86" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D86" s="20"/>
+      <c r="E86" s="20"/>
+      <c r="F86" s="20"/>
+      <c r="G86" s="20"/>
+      <c r="H86" s="20"/>
+      <c r="I86" s="20"/>
+      <c r="J86" s="20"/>
+      <c r="K86" s="20"/>
+      <c r="L86" s="20"/>
+      <c r="M86" s="20"/>
+      <c r="N86" s="20"/>
+      <c r="O86" s="20"/>
+      <c r="P86" s="20"/>
+      <c r="Q86" s="20"/>
+      <c r="R86" s="20"/>
+      <c r="S86" s="20"/>
+      <c r="T86" s="20"/>
+      <c r="U86" s="20"/>
+      <c r="V86" s="20"/>
+      <c r="W86" s="20"/>
+      <c r="X86" s="20"/>
+      <c r="Y86" s="20"/>
+      <c r="Z86" s="20"/>
+      <c r="AA86" s="20"/>
+      <c r="AB86" s="20"/>
+      <c r="AC86" s="20"/>
+      <c r="AD86" s="20"/>
+      <c r="AE86" s="20"/>
+      <c r="AF86" s="20"/>
+      <c r="AG86" s="20"/>
+      <c r="AH86" s="20"/>
+      <c r="AI86" s="20"/>
+      <c r="AJ86" s="20"/>
+      <c r="AK86" s="20"/>
+      <c r="AL86" s="20"/>
+      <c r="AM86" s="20"/>
+      <c r="AN86" s="20"/>
+      <c r="AO86" s="20"/>
+      <c r="AP86" s="20"/>
+      <c r="AQ86" s="20"/>
+      <c r="AR86" s="20"/>
+      <c r="AS86" s="20"/>
+      <c r="AT86" s="20"/>
+      <c r="AU86" s="20"/>
+      <c r="AV86" s="20"/>
+      <c r="AW86" s="20"/>
+      <c r="AX86" s="20"/>
+      <c r="AY86" s="20"/>
+      <c r="AZ86" s="20"/>
+      <c r="BA86" s="20"/>
+      <c r="BB86" s="20"/>
+      <c r="BC86" s="20"/>
+      <c r="BD86" s="20"/>
+      <c r="BE86" s="20"/>
+      <c r="BF86" s="20"/>
+      <c r="BG86" s="20"/>
+      <c r="BH86" s="20"/>
+      <c r="BI86" s="20"/>
+      <c r="BJ86" s="20"/>
+      <c r="BK86" s="20"/>
+      <c r="BL86" s="20"/>
+      <c r="BM86" s="20"/>
+      <c r="BN86" s="20"/>
+      <c r="BO86" s="20"/>
+      <c r="BP86" s="20"/>
+      <c r="BQ86" s="20"/>
+      <c r="BR86" s="20"/>
+      <c r="BS86" s="20"/>
+      <c r="BT86" s="20"/>
+      <c r="BU86" s="20"/>
+      <c r="BV86" s="20"/>
+      <c r="BW86" s="20"/>
+      <c r="BX86" s="20"/>
+      <c r="BY86" s="20"/>
+      <c r="BZ86" s="20"/>
+      <c r="CA86" s="20"/>
+      <c r="CB86" s="20"/>
+      <c r="CC86" s="20"/>
+      <c r="CD86" s="20"/>
+      <c r="CE86" s="20"/>
+      <c r="CF86" s="20"/>
+      <c r="CG86" s="20"/>
+      <c r="CH86" s="20"/>
+      <c r="CI86" s="20"/>
+      <c r="CJ86" s="20"/>
+      <c r="CK86" s="20"/>
+      <c r="CL86" s="20"/>
+      <c r="CM86" s="20"/>
+      <c r="CN86" s="20"/>
+      <c r="CO86" s="20"/>
+      <c r="CP86" s="20"/>
+      <c r="CQ86" s="20"/>
+      <c r="CR86" s="20"/>
+      <c r="CS86" s="20"/>
+      <c r="CT86" s="20"/>
+      <c r="CU86" s="20"/>
+      <c r="CV86" s="20"/>
+      <c r="CW86" s="20"/>
+      <c r="CX86" s="20"/>
+      <c r="CY86" s="20"/>
+    </row>
+    <row r="87" spans="1:103" s="28" customFormat="1" ht="15.5">
+      <c r="A87" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="B87" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C87" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D87" s="20"/>
+      <c r="E87" s="20"/>
+      <c r="F87" s="20"/>
+      <c r="G87" s="20"/>
+      <c r="H87" s="20"/>
+      <c r="I87" s="20"/>
+      <c r="J87" s="20"/>
+      <c r="K87" s="20"/>
+      <c r="L87" s="20"/>
+      <c r="M87" s="20"/>
+      <c r="N87" s="20"/>
+      <c r="O87" s="20"/>
+      <c r="P87" s="20"/>
+      <c r="Q87" s="20"/>
+      <c r="R87" s="20"/>
+      <c r="S87" s="20"/>
+      <c r="T87" s="20"/>
+      <c r="U87" s="20"/>
+      <c r="V87" s="20"/>
+      <c r="W87" s="20"/>
+      <c r="X87" s="20"/>
+      <c r="Y87" s="20"/>
+      <c r="Z87" s="20"/>
+      <c r="AA87" s="20"/>
+      <c r="AB87" s="20"/>
+      <c r="AC87" s="20"/>
+      <c r="AD87" s="20"/>
+      <c r="AE87" s="20"/>
+      <c r="AF87" s="20"/>
+      <c r="AG87" s="20"/>
+      <c r="AH87" s="20"/>
+      <c r="AI87" s="20"/>
+      <c r="AJ87" s="20"/>
+      <c r="AK87" s="20"/>
+      <c r="AL87" s="20"/>
+      <c r="AM87" s="20"/>
+      <c r="AN87" s="20"/>
+      <c r="AO87" s="20"/>
+      <c r="AP87" s="20"/>
+      <c r="AQ87" s="20"/>
+      <c r="AR87" s="20"/>
+      <c r="AS87" s="20"/>
+      <c r="AT87" s="20"/>
+      <c r="AU87" s="20"/>
+      <c r="AV87" s="20"/>
+      <c r="AW87" s="20"/>
+      <c r="AX87" s="20"/>
+      <c r="AY87" s="20"/>
+      <c r="AZ87" s="20"/>
+      <c r="BA87" s="20"/>
+      <c r="BB87" s="20"/>
+      <c r="BC87" s="20"/>
+      <c r="BD87" s="20"/>
+      <c r="BE87" s="20"/>
+      <c r="BF87" s="20"/>
+      <c r="BG87" s="20"/>
+      <c r="BH87" s="20"/>
+      <c r="BI87" s="20"/>
+      <c r="BJ87" s="20"/>
+      <c r="BK87" s="20"/>
+      <c r="BL87" s="20"/>
+      <c r="BM87" s="20"/>
+      <c r="BN87" s="20"/>
+      <c r="BO87" s="20"/>
+      <c r="BP87" s="20"/>
+      <c r="BQ87" s="20"/>
+      <c r="BR87" s="20"/>
+      <c r="BS87" s="20"/>
+      <c r="BT87" s="20"/>
+      <c r="BU87" s="20"/>
+      <c r="BV87" s="20"/>
+      <c r="BW87" s="20"/>
+      <c r="BX87" s="20"/>
+      <c r="BY87" s="20"/>
+      <c r="BZ87" s="20"/>
+      <c r="CA87" s="20"/>
+      <c r="CB87" s="20"/>
+      <c r="CC87" s="20"/>
+      <c r="CD87" s="20"/>
+      <c r="CE87" s="20"/>
+      <c r="CF87" s="20"/>
+      <c r="CG87" s="20"/>
+      <c r="CH87" s="20"/>
+      <c r="CI87" s="20"/>
+      <c r="CJ87" s="20"/>
+      <c r="CK87" s="20"/>
+      <c r="CL87" s="20"/>
+      <c r="CM87" s="20"/>
+      <c r="CN87" s="20"/>
+      <c r="CO87" s="20"/>
+      <c r="CP87" s="20"/>
+      <c r="CQ87" s="20"/>
+      <c r="CR87" s="20"/>
+      <c r="CS87" s="20"/>
+      <c r="CT87" s="20"/>
+      <c r="CU87" s="20"/>
+      <c r="CV87" s="20"/>
+      <c r="CW87" s="20"/>
+      <c r="CX87" s="20"/>
+      <c r="CY87" s="20"/>
+    </row>
+    <row r="88" spans="1:103" s="28" customFormat="1" ht="15.5">
+      <c r="A88" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="B88" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C88" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D88" s="20"/>
+      <c r="E88" s="20"/>
+      <c r="F88" s="20"/>
+      <c r="G88" s="20"/>
+      <c r="H88" s="20"/>
+      <c r="I88" s="20"/>
+      <c r="J88" s="20"/>
+      <c r="K88" s="20"/>
+      <c r="L88" s="20"/>
+      <c r="M88" s="20"/>
+      <c r="N88" s="20"/>
+      <c r="O88" s="20"/>
+      <c r="P88" s="20"/>
+      <c r="Q88" s="20"/>
+      <c r="R88" s="20"/>
+      <c r="S88" s="20"/>
+      <c r="T88" s="20"/>
+      <c r="U88" s="20"/>
+      <c r="V88" s="20"/>
+      <c r="W88" s="20"/>
+      <c r="X88" s="20"/>
+      <c r="Y88" s="20"/>
+      <c r="Z88" s="20"/>
+      <c r="AA88" s="20"/>
+      <c r="AB88" s="20"/>
+      <c r="AC88" s="20"/>
+      <c r="AD88" s="20"/>
+      <c r="AE88" s="20"/>
+      <c r="AF88" s="20"/>
+      <c r="AG88" s="20"/>
+      <c r="AH88" s="20"/>
+      <c r="AI88" s="20"/>
+      <c r="AJ88" s="20"/>
+      <c r="AK88" s="20"/>
+      <c r="AL88" s="20"/>
+      <c r="AM88" s="20"/>
+      <c r="AN88" s="20"/>
+      <c r="AO88" s="20"/>
+      <c r="AP88" s="20"/>
+      <c r="AQ88" s="20"/>
+      <c r="AR88" s="20"/>
+      <c r="AS88" s="20"/>
+      <c r="AT88" s="20"/>
+      <c r="AU88" s="20"/>
+      <c r="AV88" s="20"/>
+      <c r="AW88" s="20"/>
+      <c r="AX88" s="20"/>
+      <c r="AY88" s="20"/>
+      <c r="AZ88" s="20"/>
+      <c r="BA88" s="20"/>
+      <c r="BB88" s="20"/>
+      <c r="BC88" s="20"/>
+      <c r="BD88" s="20"/>
+      <c r="BE88" s="20"/>
+      <c r="BF88" s="20"/>
+      <c r="BG88" s="20"/>
+      <c r="BH88" s="20"/>
+      <c r="BI88" s="20"/>
+      <c r="BJ88" s="20"/>
+      <c r="BK88" s="20"/>
+      <c r="BL88" s="20"/>
+      <c r="BM88" s="20"/>
+      <c r="BN88" s="20"/>
+      <c r="BO88" s="20"/>
+      <c r="BP88" s="20"/>
+      <c r="BQ88" s="20"/>
+      <c r="BR88" s="20"/>
+      <c r="BS88" s="20"/>
+      <c r="BT88" s="20"/>
+      <c r="BU88" s="20"/>
+      <c r="BV88" s="20"/>
+      <c r="BW88" s="20"/>
+      <c r="BX88" s="20"/>
+      <c r="BY88" s="20"/>
+      <c r="BZ88" s="20"/>
+      <c r="CA88" s="20"/>
+      <c r="CB88" s="20"/>
+      <c r="CC88" s="20"/>
+      <c r="CD88" s="20"/>
+      <c r="CE88" s="20"/>
+      <c r="CF88" s="20"/>
+      <c r="CG88" s="20"/>
+      <c r="CH88" s="20"/>
+      <c r="CI88" s="20"/>
+      <c r="CJ88" s="20"/>
+      <c r="CK88" s="20"/>
+      <c r="CL88" s="20"/>
+      <c r="CM88" s="20"/>
+      <c r="CN88" s="20"/>
+      <c r="CO88" s="20"/>
+      <c r="CP88" s="20"/>
+      <c r="CQ88" s="20"/>
+      <c r="CR88" s="20"/>
+      <c r="CS88" s="20"/>
+      <c r="CT88" s="20"/>
+      <c r="CU88" s="20"/>
+      <c r="CV88" s="20"/>
+      <c r="CW88" s="20"/>
+      <c r="CX88" s="20"/>
+      <c r="CY88" s="20"/>
+    </row>
+    <row r="89" spans="1:103" s="28" customFormat="1" ht="15.5">
+      <c r="A89" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="B89" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C89" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D89" s="20"/>
+      <c r="E89" s="20"/>
+      <c r="F89" s="20"/>
+      <c r="G89" s="20"/>
+      <c r="H89" s="20"/>
+      <c r="I89" s="20"/>
+      <c r="J89" s="20"/>
+      <c r="K89" s="20"/>
+      <c r="L89" s="20"/>
+      <c r="M89" s="20"/>
+      <c r="N89" s="20"/>
+      <c r="O89" s="20"/>
+      <c r="P89" s="20"/>
+      <c r="Q89" s="20"/>
+      <c r="R89" s="20"/>
+      <c r="S89" s="20"/>
+      <c r="T89" s="20"/>
+      <c r="U89" s="20"/>
+      <c r="V89" s="20"/>
+      <c r="W89" s="20"/>
+      <c r="X89" s="20"/>
+      <c r="Y89" s="20"/>
+      <c r="Z89" s="20"/>
+      <c r="AA89" s="20"/>
+      <c r="AB89" s="20"/>
+      <c r="AC89" s="20"/>
+      <c r="AD89" s="20"/>
+      <c r="AE89" s="20"/>
+      <c r="AF89" s="20"/>
+      <c r="AG89" s="20"/>
+      <c r="AH89" s="20"/>
+      <c r="AI89" s="20"/>
+      <c r="AJ89" s="20"/>
+      <c r="AK89" s="20"/>
+      <c r="AL89" s="20"/>
+      <c r="AM89" s="20"/>
+      <c r="AN89" s="20"/>
+      <c r="AO89" s="20"/>
+      <c r="AP89" s="20"/>
+      <c r="AQ89" s="20"/>
+      <c r="AR89" s="20"/>
+      <c r="AS89" s="20"/>
+      <c r="AT89" s="20"/>
+      <c r="AU89" s="20"/>
+      <c r="AV89" s="20"/>
+      <c r="AW89" s="20"/>
+      <c r="AX89" s="20"/>
+      <c r="AY89" s="20"/>
+      <c r="AZ89" s="20"/>
+      <c r="BA89" s="20"/>
+      <c r="BB89" s="20"/>
+      <c r="BC89" s="20"/>
+      <c r="BD89" s="20"/>
+      <c r="BE89" s="20"/>
+      <c r="BF89" s="20"/>
+      <c r="BG89" s="20"/>
+      <c r="BH89" s="20"/>
+      <c r="BI89" s="20"/>
+      <c r="BJ89" s="20"/>
+      <c r="BK89" s="20"/>
+      <c r="BL89" s="20"/>
+      <c r="BM89" s="20"/>
+      <c r="BN89" s="20"/>
+      <c r="BO89" s="20"/>
+      <c r="BP89" s="20"/>
+      <c r="BQ89" s="20"/>
+      <c r="BR89" s="20"/>
+      <c r="BS89" s="20"/>
+      <c r="BT89" s="20"/>
+      <c r="BU89" s="20"/>
+      <c r="BV89" s="20"/>
+      <c r="BW89" s="20"/>
+      <c r="BX89" s="20"/>
+      <c r="BY89" s="20"/>
+      <c r="BZ89" s="20"/>
+      <c r="CA89" s="20"/>
+      <c r="CB89" s="20"/>
+      <c r="CC89" s="20"/>
+      <c r="CD89" s="20"/>
+      <c r="CE89" s="20"/>
+      <c r="CF89" s="20"/>
+      <c r="CG89" s="20"/>
+      <c r="CH89" s="20"/>
+      <c r="CI89" s="20"/>
+      <c r="CJ89" s="20"/>
+      <c r="CK89" s="20"/>
+      <c r="CL89" s="20"/>
+      <c r="CM89" s="20"/>
+      <c r="CN89" s="20"/>
+      <c r="CO89" s="20"/>
+      <c r="CP89" s="20"/>
+      <c r="CQ89" s="20"/>
+      <c r="CR89" s="20"/>
+      <c r="CS89" s="20"/>
+      <c r="CT89" s="20"/>
+      <c r="CU89" s="20"/>
+      <c r="CV89" s="20"/>
+      <c r="CW89" s="20"/>
+      <c r="CX89" s="20"/>
+      <c r="CY89" s="20"/>
+    </row>
+    <row r="90" spans="1:103" s="28" customFormat="1" ht="15.5">
+      <c r="A90" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="B90" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C90" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D90" s="20"/>
+      <c r="E90" s="20"/>
+      <c r="F90" s="20"/>
+      <c r="G90" s="20"/>
+      <c r="H90" s="20"/>
+      <c r="I90" s="20"/>
+      <c r="J90" s="20"/>
+      <c r="K90" s="20"/>
+      <c r="L90" s="20"/>
+      <c r="M90" s="20"/>
+      <c r="N90" s="20"/>
+      <c r="O90" s="20"/>
+      <c r="P90" s="20"/>
+      <c r="Q90" s="20"/>
+      <c r="R90" s="20"/>
+      <c r="S90" s="20"/>
+      <c r="T90" s="20"/>
+      <c r="U90" s="20"/>
+      <c r="V90" s="20"/>
+      <c r="W90" s="20"/>
+      <c r="X90" s="20"/>
+      <c r="Y90" s="20"/>
+      <c r="Z90" s="20"/>
+      <c r="AA90" s="20"/>
+      <c r="AB90" s="20"/>
+      <c r="AC90" s="20"/>
+      <c r="AD90" s="20"/>
+      <c r="AE90" s="20"/>
+      <c r="AF90" s="20"/>
+      <c r="AG90" s="20"/>
+      <c r="AH90" s="20"/>
+      <c r="AI90" s="20"/>
+      <c r="AJ90" s="20"/>
+      <c r="AK90" s="20"/>
+      <c r="AL90" s="20"/>
+      <c r="AM90" s="20"/>
+      <c r="AN90" s="20"/>
+      <c r="AO90" s="20"/>
+      <c r="AP90" s="20"/>
+      <c r="AQ90" s="20"/>
+      <c r="AR90" s="20"/>
+      <c r="AS90" s="20"/>
+      <c r="AT90" s="20"/>
+      <c r="AU90" s="20"/>
+      <c r="AV90" s="20"/>
+      <c r="AW90" s="20"/>
+      <c r="AX90" s="20"/>
+      <c r="AY90" s="20"/>
+      <c r="AZ90" s="20"/>
+      <c r="BA90" s="20"/>
+      <c r="BB90" s="20"/>
+      <c r="BC90" s="20"/>
+      <c r="BD90" s="20"/>
+      <c r="BE90" s="20"/>
+      <c r="BF90" s="20"/>
+      <c r="BG90" s="20"/>
+      <c r="BH90" s="20"/>
+      <c r="BI90" s="20"/>
+      <c r="BJ90" s="20"/>
+      <c r="BK90" s="20"/>
+      <c r="BL90" s="20"/>
+      <c r="BM90" s="20"/>
+      <c r="BN90" s="20"/>
+      <c r="BO90" s="20"/>
+      <c r="BP90" s="20"/>
+      <c r="BQ90" s="20"/>
+      <c r="BR90" s="20"/>
+      <c r="BS90" s="20"/>
+      <c r="BT90" s="20"/>
+      <c r="BU90" s="20"/>
+      <c r="BV90" s="20"/>
+      <c r="BW90" s="20"/>
+      <c r="BX90" s="20"/>
+      <c r="BY90" s="20"/>
+      <c r="BZ90" s="20"/>
+      <c r="CA90" s="20"/>
+      <c r="CB90" s="20"/>
+      <c r="CC90" s="20"/>
+      <c r="CD90" s="20"/>
+      <c r="CE90" s="20"/>
+      <c r="CF90" s="20"/>
+      <c r="CG90" s="20"/>
+      <c r="CH90" s="20"/>
+      <c r="CI90" s="20"/>
+      <c r="CJ90" s="20"/>
+      <c r="CK90" s="20"/>
+      <c r="CL90" s="20"/>
+      <c r="CM90" s="20"/>
+      <c r="CN90" s="20"/>
+      <c r="CO90" s="20"/>
+      <c r="CP90" s="20"/>
+      <c r="CQ90" s="20"/>
+      <c r="CR90" s="20"/>
+      <c r="CS90" s="20"/>
+      <c r="CT90" s="20"/>
+      <c r="CU90" s="20"/>
+      <c r="CV90" s="20"/>
+      <c r="CW90" s="20"/>
+      <c r="CX90" s="20"/>
+      <c r="CY90" s="20"/>
+    </row>
+    <row r="91" spans="1:103" s="28" customFormat="1" ht="15.5">
+      <c r="A91" s="6"/>
+      <c r="B91" s="6">
+        <v>79</v>
+      </c>
+      <c r="C91" s="7"/>
+      <c r="D91" s="20"/>
+      <c r="E91" s="20"/>
+      <c r="F91" s="20"/>
+      <c r="G91" s="20"/>
+      <c r="H91" s="20"/>
+      <c r="I91" s="20"/>
+      <c r="J91" s="20"/>
+      <c r="K91" s="20"/>
+      <c r="L91" s="20"/>
+      <c r="M91" s="20"/>
+      <c r="N91" s="20"/>
+      <c r="O91" s="20"/>
+      <c r="P91" s="20"/>
+      <c r="Q91" s="20"/>
+      <c r="R91" s="20"/>
+      <c r="S91" s="20"/>
+      <c r="T91" s="20"/>
+      <c r="U91" s="20"/>
+      <c r="V91" s="20"/>
+      <c r="W91" s="20"/>
+      <c r="X91" s="20"/>
+      <c r="Y91" s="20"/>
+      <c r="Z91" s="20"/>
+      <c r="AA91" s="20"/>
+      <c r="AB91" s="20"/>
+      <c r="AC91" s="20"/>
+      <c r="AD91" s="20"/>
+      <c r="AE91" s="20"/>
+      <c r="AF91" s="20"/>
+      <c r="AG91" s="20"/>
+      <c r="AH91" s="20"/>
+      <c r="AI91" s="20"/>
+      <c r="AJ91" s="20"/>
+      <c r="AK91" s="20"/>
+      <c r="AL91" s="20"/>
+      <c r="AM91" s="20"/>
+      <c r="AN91" s="20"/>
+      <c r="AO91" s="20"/>
+      <c r="AP91" s="20"/>
+      <c r="AQ91" s="20"/>
+      <c r="AR91" s="20"/>
+      <c r="AS91" s="20"/>
+      <c r="AT91" s="20"/>
+      <c r="AU91" s="20"/>
+      <c r="AV91" s="20"/>
+      <c r="AW91" s="20"/>
+      <c r="AX91" s="20"/>
+      <c r="AY91" s="20"/>
+      <c r="AZ91" s="20"/>
+      <c r="BA91" s="20"/>
+      <c r="BB91" s="20"/>
+      <c r="BC91" s="20"/>
+      <c r="BD91" s="20"/>
+      <c r="BE91" s="20"/>
+      <c r="BF91" s="20"/>
+      <c r="BG91" s="20"/>
+      <c r="BH91" s="20"/>
+      <c r="BI91" s="20"/>
+      <c r="BJ91" s="20"/>
+      <c r="BK91" s="20"/>
+      <c r="BL91" s="20"/>
+      <c r="BM91" s="20"/>
+      <c r="BN91" s="20"/>
+      <c r="BO91" s="20"/>
+      <c r="BP91" s="20"/>
+      <c r="BQ91" s="20"/>
+      <c r="BR91" s="20"/>
+      <c r="BS91" s="20"/>
+      <c r="BT91" s="20"/>
+      <c r="BU91" s="20"/>
+      <c r="BV91" s="20"/>
+      <c r="BW91" s="20"/>
+      <c r="BX91" s="20"/>
+      <c r="BY91" s="20"/>
+      <c r="BZ91" s="20"/>
+      <c r="CA91" s="20"/>
+      <c r="CB91" s="20"/>
+      <c r="CC91" s="20"/>
+      <c r="CD91" s="20"/>
+      <c r="CE91" s="20"/>
+      <c r="CF91" s="20"/>
+      <c r="CG91" s="20"/>
+      <c r="CH91" s="20"/>
+      <c r="CI91" s="20"/>
+      <c r="CJ91" s="20"/>
+      <c r="CK91" s="20"/>
+      <c r="CL91" s="20"/>
+      <c r="CM91" s="20"/>
+      <c r="CN91" s="20"/>
+      <c r="CO91" s="20"/>
+      <c r="CP91" s="20"/>
+      <c r="CQ91" s="20"/>
+      <c r="CR91" s="20"/>
+      <c r="CS91" s="20"/>
+      <c r="CT91" s="20"/>
+      <c r="CU91" s="20"/>
+      <c r="CV91" s="20"/>
+      <c r="CW91" s="20"/>
+      <c r="CX91" s="20"/>
+      <c r="CY91" s="20"/>
+    </row>
+    <row r="92" spans="1:103" s="28" customFormat="1" ht="15.5">
+      <c r="A92" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="B92" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="C92" s="30" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:103" ht="15.5">
+      <c r="A93" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B93" s="6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" ht="15.5">
-      <c r="A73" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B73" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C73" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" ht="15.5">
-      <c r="A74" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="B74" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C74" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" ht="15.5">
-      <c r="A75" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="B75" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="C75" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" ht="15.5">
-      <c r="A76" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="B76" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C76" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" ht="15.5">
-      <c r="A77" s="6"/>
-      <c r="B77" s="6"/>
-      <c r="C77" s="7"/>
-    </row>
-    <row r="78" spans="1:3" ht="15.5">
-      <c r="A78" s="27" t="s">
-        <v>164</v>
-      </c>
-      <c r="B78" s="28" t="s">
-        <v>3</v>
-      </c>
-      <c r="C78" s="28" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3">
-      <c r="A79" s="22" t="s">
-        <v>90</v>
-      </c>
-      <c r="B79" s="22"/>
-      <c r="C79" s="22"/>
-    </row>
-    <row r="80" spans="1:3">
-      <c r="A80" s="22" t="s">
-        <v>91</v>
-      </c>
-      <c r="B80" s="22"/>
-      <c r="C80" s="22"/>
-    </row>
-    <row r="81" spans="1:3">
-      <c r="A81" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="B81" s="22"/>
-      <c r="C81" s="22"/>
-    </row>
-    <row r="82" spans="1:3">
-      <c r="A82" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="B82" s="22"/>
-      <c r="C82" s="22"/>
-    </row>
-    <row r="83" spans="1:3">
-      <c r="A83" s="22" t="s">
-        <v>162</v>
-      </c>
-      <c r="B83" s="22"/>
-      <c r="C83" s="22"/>
-    </row>
-    <row r="84" spans="1:3" ht="15.5">
-      <c r="A84" s="6"/>
-      <c r="B84" s="6"/>
-      <c r="C84" s="7"/>
-    </row>
-    <row r="85" spans="1:3" ht="15.5">
-      <c r="A85" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="B85" s="28" t="s">
-        <v>3</v>
-      </c>
-      <c r="C85" s="28" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" ht="15.5">
-      <c r="A86" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B86" s="6" t="s">
+      <c r="C93" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="94" spans="1:103" ht="15.5">
+      <c r="A94" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B94" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C86" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" ht="15.5">
-      <c r="A87" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="B87" s="6" t="s">
+      <c r="C94" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="95" spans="1:103" ht="15.5">
+      <c r="A95" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B95" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C87" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" ht="15.5">
-      <c r="A88" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="B88" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="C88" s="6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" ht="15.5">
-      <c r="A89" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B89" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C89" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" ht="15.5">
-      <c r="A90" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="B90" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C90" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" ht="15.5">
-      <c r="A91" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="B91" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C91" s="22" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3">
-      <c r="A92" s="22"/>
-      <c r="B92" s="22"/>
-      <c r="C92" s="22"/>
-    </row>
-    <row r="93" spans="1:3" ht="15.5">
-      <c r="A93" s="27" t="s">
-        <v>94</v>
-      </c>
-      <c r="B93" s="28" t="s">
-        <v>3</v>
-      </c>
-      <c r="C93" s="28" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" ht="15.5">
-      <c r="A94" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="B94" s="6" t="s">
+      <c r="C95" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="96" spans="1:103" ht="15.5">
+      <c r="A96" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B96" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="C94" s="6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" ht="15.5">
-      <c r="A95" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="B95" s="6"/>
-      <c r="C95" s="6"/>
-    </row>
-    <row r="96" spans="1:3" ht="15.5">
-      <c r="A96" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="B96" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C96" s="7" t="s">
+      <c r="C96" s="6" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="15.5">
       <c r="A97" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="B97" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="B97" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C97" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98" s="20"/>
+      <c r="B98" s="20">
+        <v>84</v>
+      </c>
+      <c r="C98" s="20"/>
+    </row>
+    <row r="99" spans="1:3" ht="15.5">
+      <c r="A99" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="B99" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="C99" s="30" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" ht="15.5">
+      <c r="A100" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B100" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C100" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" ht="15.5">
+      <c r="A101" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B101" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C97" s="22" t="s">
-        <v>5</v>
+      <c r="C101" s="20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="B102" s="3">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" s="28" customFormat="1" ht="15.5">
+      <c r="A103" s="29" t="s">
+        <v>154</v>
+      </c>
+      <c r="B103" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="C103" s="30" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" ht="15.5">
+      <c r="A104" s="20" t="s">
+        <v>247</v>
+      </c>
+      <c r="B104" s="15" t="s">
+        <v>248</v>
+      </c>
+      <c r="C104" s="20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
+      <c r="A105" s="20" t="s">
+        <v>249</v>
+      </c>
+      <c r="B105" s="20" t="s">
+        <v>250</v>
+      </c>
+      <c r="C105" s="20" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
+      <c r="A106" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="B106" s="20"/>
+      <c r="C106" s="20"/>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="B107" s="3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" s="28" customFormat="1" ht="15.5">
+      <c r="A108" s="29" t="s">
+        <v>189</v>
+      </c>
+      <c r="B108" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="C108" s="30" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" ht="17.5">
+      <c r="A109" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B109" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="C109" s="14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" ht="17.5">
+      <c r="A110" s="6"/>
+      <c r="B110" s="3">
+        <v>92</v>
+      </c>
+      <c r="C110" s="14"/>
+    </row>
+    <row r="111" spans="1:3" ht="15.5">
+      <c r="A111" s="29" t="s">
+        <v>189</v>
+      </c>
+      <c r="B111" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="C111" s="30" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" ht="77.5">
+      <c r="A112" s="46" t="s">
+        <v>262</v>
+      </c>
+      <c r="B112" s="47" t="s">
+        <v>251</v>
+      </c>
+      <c r="C112" s="47" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" ht="31">
+      <c r="A113" s="46" t="s">
+        <v>263</v>
+      </c>
+      <c r="B113" s="47" t="s">
+        <v>251</v>
+      </c>
+      <c r="C113" s="47" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" ht="43.5">
+      <c r="A114" s="50" t="s">
+        <v>261</v>
+      </c>
+      <c r="B114" s="50" t="s">
+        <v>265</v>
+      </c>
+      <c r="C114" s="50" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" ht="29">
+      <c r="A115" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="B115" s="31" t="s">
+        <v>259</v>
+      </c>
+      <c r="C115" s="31" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" ht="29">
+      <c r="A116" s="49" t="s">
+        <v>268</v>
+      </c>
+      <c r="B116" s="31" t="s">
+        <v>259</v>
+      </c>
+      <c r="C116" s="31" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3">
+      <c r="A117" s="48" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3">
+      <c r="A118" s="3" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3">
+      <c r="A119" s="3" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3">
+      <c r="A120" s="3" t="s">
+        <v>267</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A65" r:id="rId1" display="https://leetcode.com/problems/spiral-matrix/" xr:uid="{A640B7C5-B7F4-449D-8CD0-BD7DA7F352C7}"/>
+    <hyperlink ref="A71" r:id="rId1" display="https://leetcode.com/problems/spiral-matrix/" xr:uid="{A640B7C5-B7F4-449D-8CD0-BD7DA7F352C7}"/>
+    <hyperlink ref="A117" r:id="rId2" xr:uid="{203B36E7-B56F-4BB0-94AB-82039AC507CC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -2527,7 +3793,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2641,7 +3907,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B3243EB-6E59-4D2E-A4B5-668F384EC9FD}">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -2654,107 +3920,107 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="35" t="s">
-        <v>200</v>
+      <c r="B1" s="21" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="37" t="s">
-        <v>192</v>
-      </c>
-      <c r="B2" s="38" t="s">
+      <c r="A2" s="23" t="s">
+        <v>181</v>
+      </c>
+      <c r="B2" s="24" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="37" t="s">
-        <v>104</v>
-      </c>
-      <c r="B3" s="36" t="s">
+      <c r="A3" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" s="22" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="37" t="s">
-        <v>194</v>
-      </c>
-      <c r="B4" s="36" t="s">
+      <c r="A4" s="23" t="s">
+        <v>183</v>
+      </c>
+      <c r="B4" s="22" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="37" t="s">
-        <v>201</v>
-      </c>
-      <c r="B5" s="36" t="s">
+      <c r="A5" s="23" t="s">
+        <v>186</v>
+      </c>
+      <c r="B5" s="22" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="22" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="37" t="s">
-        <v>195</v>
-      </c>
-      <c r="B7" s="36" t="s">
+      <c r="A7" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="B7" s="22" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="22" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="37" t="s">
-        <v>103</v>
-      </c>
-      <c r="B9" s="36" t="s">
+      <c r="A9" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="B9" s="22" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="37" t="s">
-        <v>193</v>
-      </c>
-      <c r="B10" s="36" t="s">
+      <c r="A10" s="23" t="s">
+        <v>182</v>
+      </c>
+      <c r="B10" s="22" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="20" t="s">
-        <v>191</v>
+      <c r="A11" s="18" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="20" t="s">
-        <v>195</v>
+      <c r="A14" s="18" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="21" t="s">
+      <c r="A15" s="19" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:1">
-      <c r="A19" s="20" t="s">
+      <c r="A19" s="18" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:1">
-      <c r="A20" s="20" t="s">
+      <c r="A20" s="18" t="s">
         <v>31</v>
       </c>
     </row>
@@ -2765,11 +4031,201 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14C6AA22-0ACA-4333-BF00-C3D9D81BC897}">
+  <dimension ref="A1:A38"/>
+  <sheetViews>
+    <sheetView topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="115.08984375" style="3" customWidth="1"/>
+    <col min="2" max="16384" width="8.7265625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="16.5">
+      <c r="A1" s="26" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="16.5">
+      <c r="A2" s="27" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="16.5">
+      <c r="A3" s="27" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="10"/>
+    </row>
+    <row r="5" spans="1:1" ht="16.5">
+      <c r="A5" s="26" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="16.5">
+      <c r="A6" s="27" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="10"/>
+    </row>
+    <row r="8" spans="1:1" ht="16.5">
+      <c r="A8" s="26" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="16.5">
+      <c r="A9" s="27" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="16.5">
+      <c r="A10" s="27" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" s="10"/>
+    </row>
+    <row r="12" spans="1:1" ht="16.5">
+      <c r="A12" s="26" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="16.5">
+      <c r="A13" s="27" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="16.5">
+      <c r="A14" s="27" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" s="10"/>
+    </row>
+    <row r="16" spans="1:1" ht="16.5">
+      <c r="A16" s="26" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="16.5">
+      <c r="A17" s="27" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="10"/>
+    </row>
+    <row r="19" spans="1:1" ht="16.5">
+      <c r="A19" s="26" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="16.5">
+      <c r="A20" s="27" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="10"/>
+    </row>
+    <row r="22" spans="1:1" ht="16.5">
+      <c r="A22" s="26" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" ht="16.5">
+      <c r="A23" s="27" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" ht="16.5">
+      <c r="A24" s="27" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="10"/>
+    </row>
+    <row r="26" spans="1:1" ht="16.5">
+      <c r="A26" s="26" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" ht="16.5">
+      <c r="A27" s="27" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" s="10"/>
+    </row>
+    <row r="29" spans="1:1" ht="16.5">
+      <c r="A29" s="26" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" ht="16.5">
+      <c r="A30" s="27" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" s="10"/>
+    </row>
+    <row r="32" spans="1:1" ht="16.5">
+      <c r="A32" s="26" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" ht="16.5">
+      <c r="A33" s="27" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="16.5">
+      <c r="A34" s="27" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" s="10"/>
+    </row>
+    <row r="36" spans="1:1" ht="16.5">
+      <c r="A36" s="27" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" ht="16.5">
+      <c r="A37" s="26" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" ht="16.5">
+      <c r="A38" s="27" t="s">
+        <v>217</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{074645F1-233C-463D-8568-0C05807C08A7}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2782,220 +4238,282 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>126</v>
-      </c>
       <c r="D1" s="4" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="3" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="3" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="3" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="3" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="3" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="3" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="3" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="3" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="3" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="3" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="3" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="3" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="3" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="3" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>145</v>
+        <v>118</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -3004,12 +4522,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B46DFE2-7A24-40F6-8A69-02B447E25E43}">
   <dimension ref="A1:A25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -3018,128 +4536,128 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="18" t="s">
-        <v>168</v>
+      <c r="A1" s="16" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
     </row>
     <row r="25" spans="1:1">
-      <c r="A25" s="19" t="s">
-        <v>190</v>
+      <c r="A25" s="17" t="s">
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -3151,74 +4669,79 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF65113D-2401-4C4D-853C-11C404BE93F2}">
-  <dimension ref="A1:E10"/>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63473194-51D8-4BE2-904B-37C367684259}">
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="66.6328125" style="32" customWidth="1"/>
+    <col min="2" max="2" width="35.81640625" style="32" customWidth="1"/>
+    <col min="3" max="3" width="30.26953125" style="32" customWidth="1"/>
+    <col min="4" max="16384" width="8.7265625" style="32"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1">
-        <v>110000</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2">
-        <v>18000</v>
-      </c>
-      <c r="D2">
-        <v>25500</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3">
-        <v>10000</v>
-      </c>
-      <c r="D3">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4">
-        <v>28000</v>
-      </c>
-      <c r="D4">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="D5">
-        <v>1400</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="D6">
-        <v>9700</v>
-      </c>
-      <c r="E6">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="D7">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="D9">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="D10">
-        <v>5000</v>
+    <row r="1" spans="1:3">
+      <c r="A1" s="33" t="s">
+        <v>220</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>222</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="29">
+      <c r="A2" s="32" t="s">
+        <v>221</v>
+      </c>
+      <c r="B2" s="32">
+        <v>62000</v>
+      </c>
+      <c r="C2" s="34" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="29">
+      <c r="A3" s="32" t="s">
+        <v>225</v>
+      </c>
+      <c r="B3" s="32">
+        <v>62500</v>
+      </c>
+      <c r="C3" s="34" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="43.5">
+      <c r="A4" s="34" t="s">
+        <v>230</v>
+      </c>
+      <c r="B4" s="32" t="s">
+        <v>231</v>
+      </c>
+      <c r="C4" s="34" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="32" t="s">
+        <v>232</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>233</v>
+      </c>
+      <c r="C5" s="35" t="s">
+        <v>234</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>